<commit_message>
atualização para análise de SIF
</commit_message>
<xml_diff>
--- a/output/semivariogram-models-xch4.xlsx
+++ b/output/semivariogram-models-xch4.xlsx
@@ -351,13 +351,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1"/>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>c0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>c0_c1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>gde</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>rss</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>2015</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>242.7104</v>
+      </c>
+      <c r="E2">
+        <v>665.8231</v>
+      </c>
+      <c r="F2">
+        <v>282.15</v>
+      </c>
+      <c r="G2">
+        <v>0.3645268540547782</v>
+      </c>
+      <c r="H2">
+        <v>159021056.9176</v>
+      </c>
+      <c r="I2">
+        <v>-5.6901</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>